<commit_message>
atualização da planilha de risco 01
</commit_message>
<xml_diff>
--- a/documentação/Planilha de risco.xlsx
+++ b/documentação/Planilha de risco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\BandTec\1º Semestre\Pesquisa e Inovação\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micazev/paiotnela/documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED234DCB-B70C-4568-87BB-BC8610D8128E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB52F2D2-0B67-8E4F-8386-825636169C80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8DD065CF-51B5-4F91-8D2E-2B72349E3D0A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8DD065CF-51B5-4F91-8D2E-2B72349E3D0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>idRisco</t>
   </si>
@@ -102,14 +102,29 @@
     <t>Pois é um fator incontrolável e temos  que aceitar.</t>
   </si>
   <si>
-    <t>Caso haja erro com a conexão, faremos os processos até solucionar.</t>
+    <t>Todos os membros verificarem a conexão antes de ligar o arduíno</t>
+  </si>
+  <si>
+    <t>Manter arquivo dentro da pasta do projeto com instruções de como mexer no git</t>
+  </si>
+  <si>
+    <t>Manter contato constante com os professores, buscando feedback</t>
+  </si>
+  <si>
+    <t>Caso haja erro com a conexão, repetiremos os processos até solucionar o erro.</t>
+  </si>
+  <si>
+    <t>Botões e links quebrados no site</t>
+  </si>
+  <si>
+    <t>Testar todas as funcionalidades do site antes da apresentação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,23 +133,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Exo 2 Extra Light"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Exo 2 Extra Bold"/>
-      <family val="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Exo 2 Extra Light"/>
-      <family val="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,28 +166,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -497,143 +497,179 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="39.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="14" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Alteração e finalização da Planilha de Risco
</commit_message>
<xml_diff>
--- a/documentação/Planilha de risco.xlsx
+++ b/documentação/Planilha de risco.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micazev/paiotnela/documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\paiotnela\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB52F2D2-0B67-8E4F-8386-825636169C80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95370E9-7628-4B7D-A3CF-84A4D9451E03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8DD065CF-51B5-4F91-8D2E-2B72349E3D0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8DD065CF-51B5-4F91-8D2E-2B72349E3D0A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha de Risco" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="31">
   <si>
     <t>idRisco</t>
   </si>
@@ -118,13 +118,19 @@
   </si>
   <si>
     <t>Testar todas as funcionalidades do site antes da apresentação</t>
+  </si>
+  <si>
+    <t>Imediato</t>
+  </si>
+  <si>
+    <t>Uma semana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,23 +141,35 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Exo 2"/>
+      <family val="3"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Exo 2"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Exo 2 Extra Bold"/>
+      <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -166,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -174,11 +192,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -198,7 +219,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -497,53 +518,53 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="37.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="2"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -552,20 +573,21 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -574,20 +596,24 @@
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -596,20 +622,24 @@
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="1">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -618,20 +648,24 @@
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -640,20 +674,24 @@
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="1">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -662,14 +700,18 @@
       <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Doc das Sprints semanais
</commit_message>
<xml_diff>
--- a/documentação/Planilha de risco.xlsx
+++ b/documentação/Planilha de risco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\paiotnela\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95370E9-7628-4B7D-A3CF-84A4D9451E03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8E679A-1F97-4CAC-8E34-2FC39B3398D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8DD065CF-51B5-4F91-8D2E-2B72349E3D0A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>idRisco</t>
   </si>
@@ -518,7 +518,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>